<commit_message>
case33. Market data. Update.
</commit_message>
<xml_diff>
--- a/data/CS1/CS7_market_data.xlsx
+++ b/data/CS1/CS7_market_data.xlsx
@@ -8,18 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\grid_management_tools\data\CS1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1959380-7013-4A51-B5A4-25B962D347DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E86D2D1E-242C-4F73-B48E-735B108440BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-15195" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-15195" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
     <sheet name="Cp" sheetId="2" r:id="rId2"/>
     <sheet name="Flex" sheetId="18" r:id="rId3"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId4"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -41,24 +38,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
     <t>NumScenarios</t>
   </si>
   <si>
     <t>Scenario</t>
-  </si>
-  <si>
-    <t>Value</t>
-  </si>
-  <si>
-    <t>Active Power</t>
-  </si>
-  <si>
-    <t>Growth factors (cumul.)</t>
-  </si>
-  <si>
-    <t>Flexibility</t>
   </si>
 </sst>
 </file>
@@ -113,526 +98,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="Main"/>
-      <sheetName val="Energy, Winter"/>
-      <sheetName val="Energy, Spring"/>
-      <sheetName val="Energy, Summer"/>
-      <sheetName val="Energy, Autumn"/>
-      <sheetName val="Flexibility, Winter"/>
-      <sheetName val="Flexibility, Spring"/>
-      <sheetName val="Flexibility, Summer"/>
-      <sheetName val="Flexibility, Autumn"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="B1">
-            <v>2025</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="1">
-        <row r="2">
-          <cell r="B2">
-            <v>91.75</v>
-          </cell>
-          <cell r="C2">
-            <v>86.18</v>
-          </cell>
-          <cell r="D2">
-            <v>82.1</v>
-          </cell>
-          <cell r="E2">
-            <v>80</v>
-          </cell>
-          <cell r="F2">
-            <v>79.599999999999994</v>
-          </cell>
-          <cell r="G2">
-            <v>81.099999999999994</v>
-          </cell>
-          <cell r="H2">
-            <v>85.91</v>
-          </cell>
-          <cell r="I2">
-            <v>102.05</v>
-          </cell>
-          <cell r="J2">
-            <v>113.84</v>
-          </cell>
-          <cell r="K2">
-            <v>110</v>
-          </cell>
-          <cell r="L2">
-            <v>97.63</v>
-          </cell>
-          <cell r="M2">
-            <v>86.18</v>
-          </cell>
-          <cell r="N2">
-            <v>83.89</v>
-          </cell>
-          <cell r="O2">
-            <v>82.18</v>
-          </cell>
-          <cell r="P2">
-            <v>83</v>
-          </cell>
-          <cell r="Q2">
-            <v>85</v>
-          </cell>
-          <cell r="R2">
-            <v>97.63</v>
-          </cell>
-          <cell r="S2">
-            <v>118.5</v>
-          </cell>
-          <cell r="T2">
-            <v>128.93</v>
-          </cell>
-          <cell r="U2">
-            <v>132.31</v>
-          </cell>
-          <cell r="V2">
-            <v>117.93</v>
-          </cell>
-          <cell r="W2">
-            <v>108.33</v>
-          </cell>
-          <cell r="X2">
-            <v>100</v>
-          </cell>
-          <cell r="Y2">
-            <v>93.26</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>88.98</v>
-          </cell>
-          <cell r="C3">
-            <v>86.45</v>
-          </cell>
-          <cell r="D3">
-            <v>84.99</v>
-          </cell>
-          <cell r="E3">
-            <v>83</v>
-          </cell>
-          <cell r="F3">
-            <v>83.14</v>
-          </cell>
-          <cell r="G3">
-            <v>85</v>
-          </cell>
-          <cell r="H3">
-            <v>89</v>
-          </cell>
-          <cell r="I3">
-            <v>100</v>
-          </cell>
-          <cell r="J3">
-            <v>104.77</v>
-          </cell>
-          <cell r="K3">
-            <v>105</v>
-          </cell>
-          <cell r="L3">
-            <v>100</v>
-          </cell>
-          <cell r="M3">
-            <v>94.58</v>
-          </cell>
-          <cell r="N3">
-            <v>92</v>
-          </cell>
-          <cell r="O3">
-            <v>91.78</v>
-          </cell>
-          <cell r="P3">
-            <v>90.1</v>
-          </cell>
-          <cell r="Q3">
-            <v>92.01</v>
-          </cell>
-          <cell r="R3">
-            <v>100.98</v>
-          </cell>
-          <cell r="S3">
-            <v>107.1</v>
-          </cell>
-          <cell r="T3">
-            <v>126</v>
-          </cell>
-          <cell r="U3">
-            <v>119.47</v>
-          </cell>
-          <cell r="V3">
-            <v>110</v>
-          </cell>
-          <cell r="W3">
-            <v>102.26</v>
-          </cell>
-          <cell r="X3">
-            <v>98</v>
-          </cell>
-          <cell r="Y3">
-            <v>95.49</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>92.33</v>
-          </cell>
-          <cell r="C4">
-            <v>90.12</v>
-          </cell>
-          <cell r="D4">
-            <v>87.01</v>
-          </cell>
-          <cell r="E4">
-            <v>85.8</v>
-          </cell>
-          <cell r="F4">
-            <v>85</v>
-          </cell>
-          <cell r="G4">
-            <v>86.3</v>
-          </cell>
-          <cell r="H4">
-            <v>95</v>
-          </cell>
-          <cell r="I4">
-            <v>103.94</v>
-          </cell>
-          <cell r="J4">
-            <v>121.4</v>
-          </cell>
-          <cell r="K4">
-            <v>121.4</v>
-          </cell>
-          <cell r="L4">
-            <v>105.38</v>
-          </cell>
-          <cell r="M4">
-            <v>102.97</v>
-          </cell>
-          <cell r="N4">
-            <v>99.99</v>
-          </cell>
-          <cell r="O4">
-            <v>98.5</v>
-          </cell>
-          <cell r="P4">
-            <v>94.76</v>
-          </cell>
-          <cell r="Q4">
-            <v>94.73</v>
-          </cell>
-          <cell r="R4">
-            <v>99.37</v>
-          </cell>
-          <cell r="S4">
-            <v>102.7</v>
-          </cell>
-          <cell r="T4">
-            <v>111.29</v>
-          </cell>
-          <cell r="U4">
-            <v>121.4</v>
-          </cell>
-          <cell r="V4">
-            <v>120</v>
-          </cell>
-          <cell r="W4">
-            <v>107.71</v>
-          </cell>
-          <cell r="X4">
-            <v>101.32</v>
-          </cell>
-          <cell r="Y4">
-            <v>92.68</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="2">
-        <row r="2">
-          <cell r="B2">
-            <v>44</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3">
-        <row r="2">
-          <cell r="B2">
-            <v>113.14</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="4">
-        <row r="2">
-          <cell r="B2">
-            <v>92.04</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="5">
-        <row r="2">
-          <cell r="B2">
-            <v>45.875</v>
-          </cell>
-          <cell r="C2">
-            <v>43.09</v>
-          </cell>
-          <cell r="D2">
-            <v>41.05</v>
-          </cell>
-          <cell r="E2">
-            <v>40</v>
-          </cell>
-          <cell r="F2">
-            <v>39.799999999999997</v>
-          </cell>
-          <cell r="G2">
-            <v>40.549999999999997</v>
-          </cell>
-          <cell r="H2">
-            <v>42.954999999999998</v>
-          </cell>
-          <cell r="I2">
-            <v>51.024999999999999</v>
-          </cell>
-          <cell r="J2">
-            <v>56.92</v>
-          </cell>
-          <cell r="K2">
-            <v>55</v>
-          </cell>
-          <cell r="L2">
-            <v>48.814999999999998</v>
-          </cell>
-          <cell r="M2">
-            <v>43.09</v>
-          </cell>
-          <cell r="N2">
-            <v>41.945</v>
-          </cell>
-          <cell r="O2">
-            <v>41.09</v>
-          </cell>
-          <cell r="P2">
-            <v>41.5</v>
-          </cell>
-          <cell r="Q2">
-            <v>42.5</v>
-          </cell>
-          <cell r="R2">
-            <v>48.814999999999998</v>
-          </cell>
-          <cell r="S2">
-            <v>59.25</v>
-          </cell>
-          <cell r="T2">
-            <v>64.465000000000003</v>
-          </cell>
-          <cell r="U2">
-            <v>66.155000000000001</v>
-          </cell>
-          <cell r="V2">
-            <v>58.965000000000003</v>
-          </cell>
-          <cell r="W2">
-            <v>54.164999999999999</v>
-          </cell>
-          <cell r="X2">
-            <v>50</v>
-          </cell>
-          <cell r="Y2">
-            <v>46.63</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="B3">
-            <v>44.49</v>
-          </cell>
-          <cell r="C3">
-            <v>43.225000000000001</v>
-          </cell>
-          <cell r="D3">
-            <v>42.494999999999997</v>
-          </cell>
-          <cell r="E3">
-            <v>41.5</v>
-          </cell>
-          <cell r="F3">
-            <v>41.57</v>
-          </cell>
-          <cell r="G3">
-            <v>42.5</v>
-          </cell>
-          <cell r="H3">
-            <v>44.5</v>
-          </cell>
-          <cell r="I3">
-            <v>50</v>
-          </cell>
-          <cell r="J3">
-            <v>52.384999999999998</v>
-          </cell>
-          <cell r="K3">
-            <v>52.5</v>
-          </cell>
-          <cell r="L3">
-            <v>50</v>
-          </cell>
-          <cell r="M3">
-            <v>47.29</v>
-          </cell>
-          <cell r="N3">
-            <v>46</v>
-          </cell>
-          <cell r="O3">
-            <v>45.89</v>
-          </cell>
-          <cell r="P3">
-            <v>45.05</v>
-          </cell>
-          <cell r="Q3">
-            <v>46.005000000000003</v>
-          </cell>
-          <cell r="R3">
-            <v>50.49</v>
-          </cell>
-          <cell r="S3">
-            <v>53.55</v>
-          </cell>
-          <cell r="T3">
-            <v>63</v>
-          </cell>
-          <cell r="U3">
-            <v>59.734999999999999</v>
-          </cell>
-          <cell r="V3">
-            <v>55</v>
-          </cell>
-          <cell r="W3">
-            <v>51.13</v>
-          </cell>
-          <cell r="X3">
-            <v>49</v>
-          </cell>
-          <cell r="Y3">
-            <v>47.744999999999997</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="B4">
-            <v>46.164999999999999</v>
-          </cell>
-          <cell r="C4">
-            <v>45.06</v>
-          </cell>
-          <cell r="D4">
-            <v>43.505000000000003</v>
-          </cell>
-          <cell r="E4">
-            <v>42.9</v>
-          </cell>
-          <cell r="F4">
-            <v>42.5</v>
-          </cell>
-          <cell r="G4">
-            <v>43.15</v>
-          </cell>
-          <cell r="H4">
-            <v>47.5</v>
-          </cell>
-          <cell r="I4">
-            <v>51.97</v>
-          </cell>
-          <cell r="J4">
-            <v>60.7</v>
-          </cell>
-          <cell r="K4">
-            <v>60.7</v>
-          </cell>
-          <cell r="L4">
-            <v>52.69</v>
-          </cell>
-          <cell r="M4">
-            <v>51.484999999999999</v>
-          </cell>
-          <cell r="N4">
-            <v>49.994999999999997</v>
-          </cell>
-          <cell r="O4">
-            <v>49.25</v>
-          </cell>
-          <cell r="P4">
-            <v>47.38</v>
-          </cell>
-          <cell r="Q4">
-            <v>47.365000000000002</v>
-          </cell>
-          <cell r="R4">
-            <v>49.685000000000002</v>
-          </cell>
-          <cell r="S4">
-            <v>51.35</v>
-          </cell>
-          <cell r="T4">
-            <v>55.645000000000003</v>
-          </cell>
-          <cell r="U4">
-            <v>60.7</v>
-          </cell>
-          <cell r="V4">
-            <v>60</v>
-          </cell>
-          <cell r="W4">
-            <v>53.854999999999997</v>
-          </cell>
-          <cell r="X4">
-            <v>50.66</v>
-          </cell>
-          <cell r="Y4">
-            <v>46.34</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="6">
-        <row r="2">
-          <cell r="B2">
-            <v>22</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="7">
-        <row r="2">
-          <cell r="B2">
-            <v>56.57</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="8">
-        <row r="2">
-          <cell r="B2">
-            <v>46.02</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -898,10 +363,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -931,30 +396,6 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1054,99 +495,75 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <f>'[1]Energy, Winter'!B2*Scenarios!$B$4</f>
         <v>91.75</v>
       </c>
       <c r="C2" s="2">
-        <f>'[1]Energy, Winter'!C2*Scenarios!$B$4</f>
         <v>86.18</v>
       </c>
       <c r="D2" s="2">
-        <f>'[1]Energy, Winter'!D2*Scenarios!$B$4</f>
         <v>82.1</v>
       </c>
       <c r="E2" s="2">
-        <f>'[1]Energy, Winter'!E2*Scenarios!$B$4</f>
         <v>80</v>
       </c>
       <c r="F2" s="2">
-        <f>'[1]Energy, Winter'!F2*Scenarios!$B$4</f>
         <v>79.599999999999994</v>
       </c>
       <c r="G2" s="2">
-        <f>'[1]Energy, Winter'!G2*Scenarios!$B$4</f>
         <v>81.099999999999994</v>
       </c>
       <c r="H2" s="2">
-        <f>'[1]Energy, Winter'!H2*Scenarios!$B$4</f>
         <v>85.91</v>
       </c>
       <c r="I2" s="2">
-        <f>'[1]Energy, Winter'!I2*Scenarios!$B$4</f>
         <v>102.05</v>
       </c>
       <c r="J2" s="2">
-        <f>'[1]Energy, Winter'!J2*Scenarios!$B$4</f>
         <v>113.84</v>
       </c>
       <c r="K2" s="2">
-        <f>'[1]Energy, Winter'!K2*Scenarios!$B$4</f>
         <v>110</v>
       </c>
       <c r="L2" s="2">
-        <f>'[1]Energy, Winter'!L2*Scenarios!$B$4</f>
         <v>97.63</v>
       </c>
       <c r="M2" s="2">
-        <f>'[1]Energy, Winter'!M2*Scenarios!$B$4</f>
         <v>86.18</v>
       </c>
       <c r="N2" s="2">
-        <f>'[1]Energy, Winter'!N2*Scenarios!$B$4</f>
         <v>83.89</v>
       </c>
       <c r="O2" s="2">
-        <f>'[1]Energy, Winter'!O2*Scenarios!$B$4</f>
         <v>82.18</v>
       </c>
       <c r="P2" s="2">
-        <f>'[1]Energy, Winter'!P2*Scenarios!$B$4</f>
         <v>83</v>
       </c>
       <c r="Q2" s="2">
-        <f>'[1]Energy, Winter'!Q2*Scenarios!$B$4</f>
         <v>85</v>
       </c>
       <c r="R2" s="2">
-        <f>'[1]Energy, Winter'!R2*Scenarios!$B$4</f>
         <v>97.63</v>
       </c>
       <c r="S2" s="2">
-        <f>'[1]Energy, Winter'!S2*Scenarios!$B$4</f>
         <v>118.5</v>
       </c>
       <c r="T2" s="2">
-        <f>'[1]Energy, Winter'!T2*Scenarios!$B$4</f>
         <v>128.93</v>
       </c>
       <c r="U2" s="2">
-        <f>'[1]Energy, Winter'!U2*Scenarios!$B$4</f>
         <v>132.31</v>
       </c>
       <c r="V2" s="2">
-        <f>'[1]Energy, Winter'!V2*Scenarios!$B$4</f>
         <v>117.93</v>
       </c>
       <c r="W2" s="2">
-        <f>'[1]Energy, Winter'!W2*Scenarios!$B$4</f>
         <v>108.33</v>
       </c>
       <c r="X2" s="2">
-        <f>'[1]Energy, Winter'!X2*Scenarios!$B$4</f>
         <v>100</v>
       </c>
       <c r="Y2" s="2">
-        <f>'[1]Energy, Winter'!Y2*Scenarios!$B$4</f>
         <v>93.26</v>
       </c>
     </row>
@@ -1155,99 +572,75 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <f>'[1]Energy, Winter'!B3*Scenarios!$B$4</f>
         <v>88.98</v>
       </c>
       <c r="C3" s="2">
-        <f>'[1]Energy, Winter'!C3*Scenarios!$B$4</f>
         <v>86.45</v>
       </c>
       <c r="D3" s="2">
-        <f>'[1]Energy, Winter'!D3*Scenarios!$B$4</f>
         <v>84.99</v>
       </c>
       <c r="E3" s="2">
-        <f>'[1]Energy, Winter'!E3*Scenarios!$B$4</f>
         <v>83</v>
       </c>
       <c r="F3" s="2">
-        <f>'[1]Energy, Winter'!F3*Scenarios!$B$4</f>
         <v>83.14</v>
       </c>
       <c r="G3" s="2">
-        <f>'[1]Energy, Winter'!G3*Scenarios!$B$4</f>
         <v>85</v>
       </c>
       <c r="H3" s="2">
-        <f>'[1]Energy, Winter'!H3*Scenarios!$B$4</f>
         <v>89</v>
       </c>
       <c r="I3" s="2">
-        <f>'[1]Energy, Winter'!I3*Scenarios!$B$4</f>
         <v>100</v>
       </c>
       <c r="J3" s="2">
-        <f>'[1]Energy, Winter'!J3*Scenarios!$B$4</f>
         <v>104.77</v>
       </c>
       <c r="K3" s="2">
-        <f>'[1]Energy, Winter'!K3*Scenarios!$B$4</f>
         <v>105</v>
       </c>
       <c r="L3" s="2">
-        <f>'[1]Energy, Winter'!L3*Scenarios!$B$4</f>
         <v>100</v>
       </c>
       <c r="M3" s="2">
-        <f>'[1]Energy, Winter'!M3*Scenarios!$B$4</f>
         <v>94.58</v>
       </c>
       <c r="N3" s="2">
-        <f>'[1]Energy, Winter'!N3*Scenarios!$B$4</f>
         <v>92</v>
       </c>
       <c r="O3" s="2">
-        <f>'[1]Energy, Winter'!O3*Scenarios!$B$4</f>
         <v>91.78</v>
       </c>
       <c r="P3" s="2">
-        <f>'[1]Energy, Winter'!P3*Scenarios!$B$4</f>
         <v>90.1</v>
       </c>
       <c r="Q3" s="2">
-        <f>'[1]Energy, Winter'!Q3*Scenarios!$B$4</f>
         <v>92.01</v>
       </c>
       <c r="R3" s="2">
-        <f>'[1]Energy, Winter'!R3*Scenarios!$B$4</f>
         <v>100.98</v>
       </c>
       <c r="S3" s="2">
-        <f>'[1]Energy, Winter'!S3*Scenarios!$B$4</f>
         <v>107.1</v>
       </c>
       <c r="T3" s="2">
-        <f>'[1]Energy, Winter'!T3*Scenarios!$B$4</f>
         <v>126</v>
       </c>
       <c r="U3" s="2">
-        <f>'[1]Energy, Winter'!U3*Scenarios!$B$4</f>
         <v>119.47</v>
       </c>
       <c r="V3" s="2">
-        <f>'[1]Energy, Winter'!V3*Scenarios!$B$4</f>
         <v>110</v>
       </c>
       <c r="W3" s="2">
-        <f>'[1]Energy, Winter'!W3*Scenarios!$B$4</f>
         <v>102.26</v>
       </c>
       <c r="X3" s="2">
-        <f>'[1]Energy, Winter'!X3*Scenarios!$B$4</f>
         <v>98</v>
       </c>
       <c r="Y3" s="2">
-        <f>'[1]Energy, Winter'!Y3*Scenarios!$B$4</f>
         <v>95.49</v>
       </c>
     </row>
@@ -1256,99 +649,75 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <f>'[1]Energy, Winter'!B4*Scenarios!$B$4</f>
         <v>92.33</v>
       </c>
       <c r="C4" s="2">
-        <f>'[1]Energy, Winter'!C4*Scenarios!$B$4</f>
         <v>90.12</v>
       </c>
       <c r="D4" s="2">
-        <f>'[1]Energy, Winter'!D4*Scenarios!$B$4</f>
         <v>87.01</v>
       </c>
       <c r="E4" s="2">
-        <f>'[1]Energy, Winter'!E4*Scenarios!$B$4</f>
         <v>85.8</v>
       </c>
       <c r="F4" s="2">
-        <f>'[1]Energy, Winter'!F4*Scenarios!$B$4</f>
         <v>85</v>
       </c>
       <c r="G4" s="2">
-        <f>'[1]Energy, Winter'!G4*Scenarios!$B$4</f>
         <v>86.3</v>
       </c>
       <c r="H4" s="2">
-        <f>'[1]Energy, Winter'!H4*Scenarios!$B$4</f>
         <v>95</v>
       </c>
       <c r="I4" s="2">
-        <f>'[1]Energy, Winter'!I4*Scenarios!$B$4</f>
         <v>103.94</v>
       </c>
       <c r="J4" s="2">
-        <f>'[1]Energy, Winter'!J4*Scenarios!$B$4</f>
         <v>121.4</v>
       </c>
       <c r="K4" s="2">
-        <f>'[1]Energy, Winter'!K4*Scenarios!$B$4</f>
         <v>121.4</v>
       </c>
       <c r="L4" s="2">
-        <f>'[1]Energy, Winter'!L4*Scenarios!$B$4</f>
         <v>105.38</v>
       </c>
       <c r="M4" s="2">
-        <f>'[1]Energy, Winter'!M4*Scenarios!$B$4</f>
         <v>102.97</v>
       </c>
       <c r="N4" s="2">
-        <f>'[1]Energy, Winter'!N4*Scenarios!$B$4</f>
         <v>99.99</v>
       </c>
       <c r="O4" s="2">
-        <f>'[1]Energy, Winter'!O4*Scenarios!$B$4</f>
         <v>98.5</v>
       </c>
       <c r="P4" s="2">
-        <f>'[1]Energy, Winter'!P4*Scenarios!$B$4</f>
         <v>94.76</v>
       </c>
       <c r="Q4" s="2">
-        <f>'[1]Energy, Winter'!Q4*Scenarios!$B$4</f>
         <v>94.73</v>
       </c>
       <c r="R4" s="2">
-        <f>'[1]Energy, Winter'!R4*Scenarios!$B$4</f>
         <v>99.37</v>
       </c>
       <c r="S4" s="2">
-        <f>'[1]Energy, Winter'!S4*Scenarios!$B$4</f>
         <v>102.7</v>
       </c>
       <c r="T4" s="2">
-        <f>'[1]Energy, Winter'!T4*Scenarios!$B$4</f>
         <v>111.29</v>
       </c>
       <c r="U4" s="2">
-        <f>'[1]Energy, Winter'!U4*Scenarios!$B$4</f>
         <v>121.4</v>
       </c>
       <c r="V4" s="2">
-        <f>'[1]Energy, Winter'!V4*Scenarios!$B$4</f>
         <v>120</v>
       </c>
       <c r="W4" s="2">
-        <f>'[1]Energy, Winter'!W4*Scenarios!$B$4</f>
         <v>107.71</v>
       </c>
       <c r="X4" s="2">
-        <f>'[1]Energy, Winter'!X4*Scenarios!$B$4</f>
         <v>101.32</v>
       </c>
       <c r="Y4" s="2">
-        <f>'[1]Energy, Winter'!Y4*Scenarios!$B$4</f>
         <v>92.68</v>
       </c>
     </row>
@@ -1414,8 +783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59BA0F2A-A97B-42BF-BD16-0283FFE6BEE7}">
   <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1502,99 +871,75 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <f>'[1]Flexibility, Winter'!B2*Scenarios!$B$4</f>
         <v>45.875</v>
       </c>
       <c r="C2" s="2">
-        <f>'[1]Flexibility, Winter'!C2*Scenarios!$B$4</f>
         <v>43.09</v>
       </c>
       <c r="D2" s="2">
-        <f>'[1]Flexibility, Winter'!D2*Scenarios!$B$4</f>
         <v>41.05</v>
       </c>
       <c r="E2" s="2">
-        <f>'[1]Flexibility, Winter'!E2*Scenarios!$B$4</f>
         <v>40</v>
       </c>
       <c r="F2" s="2">
-        <f>'[1]Flexibility, Winter'!F2*Scenarios!$B$4</f>
         <v>39.799999999999997</v>
       </c>
       <c r="G2" s="2">
-        <f>'[1]Flexibility, Winter'!G2*Scenarios!$B$4</f>
         <v>40.549999999999997</v>
       </c>
       <c r="H2" s="2">
-        <f>'[1]Flexibility, Winter'!H2*Scenarios!$B$4</f>
         <v>42.954999999999998</v>
       </c>
       <c r="I2" s="2">
-        <f>'[1]Flexibility, Winter'!I2*Scenarios!$B$4</f>
         <v>51.024999999999999</v>
       </c>
       <c r="J2" s="2">
-        <f>'[1]Flexibility, Winter'!J2*Scenarios!$B$4</f>
         <v>56.92</v>
       </c>
       <c r="K2" s="2">
-        <f>'[1]Flexibility, Winter'!K2*Scenarios!$B$4</f>
         <v>55</v>
       </c>
       <c r="L2" s="2">
-        <f>'[1]Flexibility, Winter'!L2*Scenarios!$B$4</f>
         <v>48.814999999999998</v>
       </c>
       <c r="M2" s="2">
-        <f>'[1]Flexibility, Winter'!M2*Scenarios!$B$4</f>
         <v>43.09</v>
       </c>
       <c r="N2" s="2">
-        <f>'[1]Flexibility, Winter'!N2*Scenarios!$B$4</f>
         <v>41.945</v>
       </c>
       <c r="O2" s="2">
-        <f>'[1]Flexibility, Winter'!O2*Scenarios!$B$4</f>
         <v>41.09</v>
       </c>
       <c r="P2" s="2">
-        <f>'[1]Flexibility, Winter'!P2*Scenarios!$B$4</f>
         <v>41.5</v>
       </c>
       <c r="Q2" s="2">
-        <f>'[1]Flexibility, Winter'!Q2*Scenarios!$B$4</f>
         <v>42.5</v>
       </c>
       <c r="R2" s="2">
-        <f>'[1]Flexibility, Winter'!R2*Scenarios!$B$4</f>
         <v>48.814999999999998</v>
       </c>
       <c r="S2" s="2">
-        <f>'[1]Flexibility, Winter'!S2*Scenarios!$B$4</f>
         <v>59.25</v>
       </c>
       <c r="T2" s="2">
-        <f>'[1]Flexibility, Winter'!T2*Scenarios!$B$4</f>
         <v>64.465000000000003</v>
       </c>
       <c r="U2" s="2">
-        <f>'[1]Flexibility, Winter'!U2*Scenarios!$B$4</f>
         <v>66.155000000000001</v>
       </c>
       <c r="V2" s="2">
-        <f>'[1]Flexibility, Winter'!V2*Scenarios!$B$4</f>
         <v>58.965000000000003</v>
       </c>
       <c r="W2" s="2">
-        <f>'[1]Flexibility, Winter'!W2*Scenarios!$B$4</f>
         <v>54.164999999999999</v>
       </c>
       <c r="X2" s="2">
-        <f>'[1]Flexibility, Winter'!X2*Scenarios!$B$4</f>
         <v>50</v>
       </c>
       <c r="Y2" s="2">
-        <f>'[1]Flexibility, Winter'!Y2*Scenarios!$B$4</f>
         <v>46.63</v>
       </c>
     </row>
@@ -1603,99 +948,75 @@
         <v>2</v>
       </c>
       <c r="B3" s="2">
-        <f>'[1]Flexibility, Winter'!B3*Scenarios!$B$4</f>
         <v>44.49</v>
       </c>
       <c r="C3" s="2">
-        <f>'[1]Flexibility, Winter'!C3*Scenarios!$B$4</f>
         <v>43.225000000000001</v>
       </c>
       <c r="D3" s="2">
-        <f>'[1]Flexibility, Winter'!D3*Scenarios!$B$4</f>
         <v>42.494999999999997</v>
       </c>
       <c r="E3" s="2">
-        <f>'[1]Flexibility, Winter'!E3*Scenarios!$B$4</f>
         <v>41.5</v>
       </c>
       <c r="F3" s="2">
-        <f>'[1]Flexibility, Winter'!F3*Scenarios!$B$4</f>
         <v>41.57</v>
       </c>
       <c r="G3" s="2">
-        <f>'[1]Flexibility, Winter'!G3*Scenarios!$B$4</f>
         <v>42.5</v>
       </c>
       <c r="H3" s="2">
-        <f>'[1]Flexibility, Winter'!H3*Scenarios!$B$4</f>
         <v>44.5</v>
       </c>
       <c r="I3" s="2">
-        <f>'[1]Flexibility, Winter'!I3*Scenarios!$B$4</f>
         <v>50</v>
       </c>
       <c r="J3" s="2">
-        <f>'[1]Flexibility, Winter'!J3*Scenarios!$B$4</f>
         <v>52.384999999999998</v>
       </c>
       <c r="K3" s="2">
-        <f>'[1]Flexibility, Winter'!K3*Scenarios!$B$4</f>
         <v>52.5</v>
       </c>
       <c r="L3" s="2">
-        <f>'[1]Flexibility, Winter'!L3*Scenarios!$B$4</f>
         <v>50</v>
       </c>
       <c r="M3" s="2">
-        <f>'[1]Flexibility, Winter'!M3*Scenarios!$B$4</f>
         <v>47.29</v>
       </c>
       <c r="N3" s="2">
-        <f>'[1]Flexibility, Winter'!N3*Scenarios!$B$4</f>
         <v>46</v>
       </c>
       <c r="O3" s="2">
-        <f>'[1]Flexibility, Winter'!O3*Scenarios!$B$4</f>
         <v>45.89</v>
       </c>
       <c r="P3" s="2">
-        <f>'[1]Flexibility, Winter'!P3*Scenarios!$B$4</f>
         <v>45.05</v>
       </c>
       <c r="Q3" s="2">
-        <f>'[1]Flexibility, Winter'!Q3*Scenarios!$B$4</f>
         <v>46.005000000000003</v>
       </c>
       <c r="R3" s="2">
-        <f>'[1]Flexibility, Winter'!R3*Scenarios!$B$4</f>
         <v>50.49</v>
       </c>
       <c r="S3" s="2">
-        <f>'[1]Flexibility, Winter'!S3*Scenarios!$B$4</f>
         <v>53.55</v>
       </c>
       <c r="T3" s="2">
-        <f>'[1]Flexibility, Winter'!T3*Scenarios!$B$4</f>
         <v>63</v>
       </c>
       <c r="U3" s="2">
-        <f>'[1]Flexibility, Winter'!U3*Scenarios!$B$4</f>
         <v>59.734999999999999</v>
       </c>
       <c r="V3" s="2">
-        <f>'[1]Flexibility, Winter'!V3*Scenarios!$B$4</f>
         <v>55</v>
       </c>
       <c r="W3" s="2">
-        <f>'[1]Flexibility, Winter'!W3*Scenarios!$B$4</f>
         <v>51.13</v>
       </c>
       <c r="X3" s="2">
-        <f>'[1]Flexibility, Winter'!X3*Scenarios!$B$4</f>
         <v>49</v>
       </c>
       <c r="Y3" s="2">
-        <f>'[1]Flexibility, Winter'!Y3*Scenarios!$B$4</f>
         <v>47.744999999999997</v>
       </c>
     </row>
@@ -1704,99 +1025,75 @@
         <v>3</v>
       </c>
       <c r="B4" s="2">
-        <f>'[1]Flexibility, Winter'!B4*Scenarios!$B$4</f>
         <v>46.164999999999999</v>
       </c>
       <c r="C4" s="2">
-        <f>'[1]Flexibility, Winter'!C4*Scenarios!$B$4</f>
         <v>45.06</v>
       </c>
       <c r="D4" s="2">
-        <f>'[1]Flexibility, Winter'!D4*Scenarios!$B$4</f>
         <v>43.505000000000003</v>
       </c>
       <c r="E4" s="2">
-        <f>'[1]Flexibility, Winter'!E4*Scenarios!$B$4</f>
         <v>42.9</v>
       </c>
       <c r="F4" s="2">
-        <f>'[1]Flexibility, Winter'!F4*Scenarios!$B$4</f>
         <v>42.5</v>
       </c>
       <c r="G4" s="2">
-        <f>'[1]Flexibility, Winter'!G4*Scenarios!$B$4</f>
         <v>43.15</v>
       </c>
       <c r="H4" s="2">
-        <f>'[1]Flexibility, Winter'!H4*Scenarios!$B$4</f>
         <v>47.5</v>
       </c>
       <c r="I4" s="2">
-        <f>'[1]Flexibility, Winter'!I4*Scenarios!$B$4</f>
         <v>51.97</v>
       </c>
       <c r="J4" s="2">
-        <f>'[1]Flexibility, Winter'!J4*Scenarios!$B$4</f>
         <v>60.7</v>
       </c>
       <c r="K4" s="2">
-        <f>'[1]Flexibility, Winter'!K4*Scenarios!$B$4</f>
         <v>60.7</v>
       </c>
       <c r="L4" s="2">
-        <f>'[1]Flexibility, Winter'!L4*Scenarios!$B$4</f>
         <v>52.69</v>
       </c>
       <c r="M4" s="2">
-        <f>'[1]Flexibility, Winter'!M4*Scenarios!$B$4</f>
         <v>51.484999999999999</v>
       </c>
       <c r="N4" s="2">
-        <f>'[1]Flexibility, Winter'!N4*Scenarios!$B$4</f>
         <v>49.994999999999997</v>
       </c>
       <c r="O4" s="2">
-        <f>'[1]Flexibility, Winter'!O4*Scenarios!$B$4</f>
         <v>49.25</v>
       </c>
       <c r="P4" s="2">
-        <f>'[1]Flexibility, Winter'!P4*Scenarios!$B$4</f>
         <v>47.38</v>
       </c>
       <c r="Q4" s="2">
-        <f>'[1]Flexibility, Winter'!Q4*Scenarios!$B$4</f>
         <v>47.365000000000002</v>
       </c>
       <c r="R4" s="2">
-        <f>'[1]Flexibility, Winter'!R4*Scenarios!$B$4</f>
         <v>49.685000000000002</v>
       </c>
       <c r="S4" s="2">
-        <f>'[1]Flexibility, Winter'!S4*Scenarios!$B$4</f>
         <v>51.35</v>
       </c>
       <c r="T4" s="2">
-        <f>'[1]Flexibility, Winter'!T4*Scenarios!$B$4</f>
         <v>55.645000000000003</v>
       </c>
       <c r="U4" s="2">
-        <f>'[1]Flexibility, Winter'!U4*Scenarios!$B$4</f>
         <v>60.7</v>
       </c>
       <c r="V4" s="2">
-        <f>'[1]Flexibility, Winter'!V4*Scenarios!$B$4</f>
         <v>60</v>
       </c>
       <c r="W4" s="2">
-        <f>'[1]Flexibility, Winter'!W4*Scenarios!$B$4</f>
         <v>53.854999999999997</v>
       </c>
       <c r="X4" s="2">
-        <f>'[1]Flexibility, Winter'!X4*Scenarios!$B$4</f>
         <v>50.66</v>
       </c>
       <c r="Y4" s="2">
-        <f>'[1]Flexibility, Winter'!Y4*Scenarios!$B$4</f>
         <v>46.34</v>
       </c>
     </row>

</xml_diff>